<commit_message>
in pom.xml added systemPropertyVariables to get values from jenkins
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSheet/HRM.xlsx
+++ b/src/test/resources/DataSheet/HRM.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esparja\Downloads\HRM_old\HRM_old\DataSheet\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14085" windowHeight="4695" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15660" windowHeight="4200"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Details" sheetId="1" r:id="rId1"/>
@@ -17,6 +12,7 @@
     <sheet name="Expenses_Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:O12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -103,7 +99,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -256,23 +252,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -308,23 +287,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -479,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>